<commit_message>
Check Date and Unit Test
</commit_message>
<xml_diff>
--- a/engine/src/test/resources/KYC.xlsx
+++ b/engine/src/test/resources/KYC.xlsx
@@ -87,7 +87,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>PEP</t>
   </si>
@@ -120,6 +120,9 @@
   </si>
   <si>
     <t>FINAL</t>
+  </si>
+  <si>
+    <t>1ER JAN</t>
   </si>
 </sst>
 </file>
@@ -189,11 +192,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
@@ -537,10 +542,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A6"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -606,6 +611,23 @@
       <c r="C6">
         <f>SUM(C2:C4)</f>
         <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="2">
+        <v>44197</v>
+      </c>
+      <c r="C9" s="3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="C10" s="2">
+        <f>B9+C9</f>
+        <v>44239</v>
       </c>
     </row>
   </sheetData>

</xml_diff>